<commit_message>
Emoji remove added LSTM dictionary size limitation SVM code fixed (MNB -> SVM) - models push
</commit_message>
<xml_diff>
--- a/data/final-data-set.xlsx
+++ b/data/final-data-set.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="538">
   <si>
     <t>World-Against-Islam Google Search Image: Islam is … bullshit, false, not a religion, a lie, the light, of the devil, wrong, founded, google, fake</t>
   </si>
@@ -1341,6 +1341,303 @@
   </si>
   <si>
     <t>"@Rasthiyaduwa ස්තුතියි රස්තා 😂"</t>
+  </si>
+  <si>
+    <t>"@Madurangakalpa1 ගහමු..පතා එකේ... දවසක..😁"</t>
+  </si>
+  <si>
+    <t>"නංගි තරහ වෙලා කියහල්ලකො... ඕක කෙල්ලට ආරංචි උනොත් කෙලින්ම නෑන පොඩ්ඩගෙ පැත්ත අරන් මාව බලයෙන් පහ කරනව කියහල්ලකො....😌"</t>
+  </si>
+  <si>
+    <t>"එක දවසක අපි නුපුරුදු සුවඳක හිත හෙමිහිට බැඳුනා අප හමුවුණු හිනැහුණු මතකය සසර පුරුදු හැඟුණා 🖤🖤🖤 — feeling loved"</t>
+  </si>
+  <si>
+    <t>"@nsadisha 😂😂😂😂 ආපු දවසක පෙනන"</t>
+  </si>
+  <si>
+    <t>"@techn0ish 😂😂😂 මේකට මොනාට් උනොත් මං ආයෙ ටුයිටර් නෑහ් 😂🤘"</t>
+  </si>
+  <si>
+    <t>"@MatiBole උදම්මිට පාරෙන් එන දවසක අනිවා එනවා ඔන්න"</t>
+  </si>
+  <si>
+    <t>"@PeirisDarshana මම හොයලා හිතලා නෑ. ඇහෙන යමක් විතරයි."</t>
+  </si>
+  <si>
+    <t>"@MatiBole ම්ම්ම්ම් බැරිවෙලාවත් සැන්ටා උනොත් මුලින්ම හොයලා දෙන්නේ ඔයාට එහෙනම්.. ☺️"</t>
+  </si>
+  <si>
+    <t>"විද්‍යාත්මක ව හිතලා කාන්තා කටයුතු හා වියලි කලාප සංවර්ධන අමාත්‍යාංශය හැදුවා. දැන් කාන්තාවන් ගේ වියලි කලාප සංවර්ධනය වෙයි මේම මේම."</t>
+  </si>
+  <si>
+    <t>"@PoDiyaa වටයක් දෙකක් දාලා බැරිම උනොත් හිස් අතින් ෆිටෝන් එකට ගිහින් ආයේ වරෙන් 😂"</t>
+  </si>
+  <si>
+    <t>"අනේ නිකන් ඉන්නව සංජු අක්කෙ 😂 ඔයාහෙ 6යිද ලිස්ට් එක 🙊🙊 ආයෙ හදන් නෑමයි මේකට මොනාහරි උනොත් 😂 https://t.co/7eoD8BRUYz"</t>
+  </si>
+  <si>
+    <t>"@AchiniHansima එහෙම උනොත් නම් ලොකු දෙයක් 😭♥️"</t>
+  </si>
+  <si>
+    <t>"@chathuranga513 ඔව් ඉතින් දෙකක් හදලත් මෙහෙම උනානෙ. මේකටත් එහෙම උනොත් ආයෙ හද න්නද ? බෑනෙ"</t>
+  </si>
+  <si>
+    <t>"සමහරු කතා කරන්නේ නිකන් ජනාධිපතිපති හිතලා කට්ටියව පත් කරනවා වගේනේ. 😂😂😂 පව් අර අහිංසකයා. 😁😂"</t>
+  </si>
+  <si>
+    <t>"@Nadeez__ හා බායි එහෙනම් 😂 මොනාහරි උනොත් බායි කියන්න වෙන්නෙත් නෑනෙ 😂😂😂😂"</t>
+  </si>
+  <si>
+    <t>"@wishawanath හහා 😂😂😂 එහෙමවත් සෙට් උනොත් තමා අපිට"</t>
+  </si>
+  <si>
+    <t>"අර්ජුන් ඇලෝසියස් හදිසියේ අසනීප වෙයි - ඩෙංගුදැයි සැක - https://t.co/8bZoOfHdHU"</t>
+  </si>
+  <si>
+    <t>"අර්ජුන් ඇලෝසියස් හදිසියේ අසනීප වෙයි - ඩෙංගුදැයි සැක - https://t.co/RkGbK2kU8K"</t>
+  </si>
+  <si>
+    <t>"@Nadeez__ නෑ නෑ නෑ 😂😂😂 පරණ එක හදාගත්තොත් ඉන්නව. මේකටත් ඒකම උනොත් එන්නෙ නෑ නෑ නෑ නෑ නෑ"</t>
+  </si>
+  <si>
+    <t>"මම මේක නැති උනොත් ආයෙ ටුයිටර් එන්නෙ නෑ 😂 https://t.co/yx0XHIdIGl"</t>
+  </si>
+  <si>
+    <t>"@Nadeez__ හා එහෙනම් 😏 ආයෙ ඉතින් මේකත් නැති උනොත් නම් හදන්නෙ නෑමයි එකක් 😂 පරණ එක හරි ගියොත් නම් 😍😍😍😍😍😍😍😍😍😍"</t>
+  </si>
+  <si>
+    <t>"මේකටත් මොනාහරි උනොත් ආයෙ ටුයිටර් එන්නෙ නෑ 😂👋"</t>
+  </si>
+  <si>
+    <t>"@Sansajran @dead_mans_creed 😂😂😂 මාත් දැම්මා එහෙම හිතලා"</t>
+  </si>
+  <si>
+    <t>"අර්ජුන් ඇලෝසියස් හදිසියේ අසනීප වෙයි - ඩෙංගුදැයි සැක https://t.co/pYURblAJDo https://t.co/pYURblAJDo"</t>
+  </si>
+  <si>
+    <t>"අර්ජුන් ඇලෝසියස් හදිසියේ අසනීප වෙයි - ඩෙංගුදැයි සැක https://t.co/LTcyrbML7T https://t.co/LTcyrbML7T"</t>
+  </si>
+  <si>
+    <t>"@Lovely_Paba @tharu__ @akhilasg @Nadeez__ පබා අපි ආයෙම දවසක කතා කරමු."</t>
+  </si>
+  <si>
+    <t>"සත්තයි දවසක ඔබ හඩනවා මම හඩන තරමටම...."</t>
+  </si>
+  <si>
+    <t>"අපි ආයේ ඒ ගැන දවසක කතා කරමු. https://t.co/Fe45fEqV12"</t>
+  </si>
+  <si>
+    <t>"@Jude_H_Fernando @tikirimaarie වැඩිම උනොත් ඇවිත් "haha" emoji එකක් දාල යාවි 😂😂"</t>
+  </si>
+  <si>
+    <t>"@sheshandj ඔයා තමා වගකියන්න ඕනෙ ඔහොම කියල මට මොනාහරි උනොත් 😏😭"</t>
+  </si>
+  <si>
+    <t>"@Rasthiyaduwa ✋😂 දවසක හාද"</t>
+  </si>
+  <si>
+    <t>"නුඹ නැතුව හිත හැදෙන් නෑ ළඟට ඇවිදින් අඬන් නෑ ලැබෙන දවසක ලැබෙනවා නම් සිතින් කිසිදින හැලෙන් නෑ.. #සිතුවිලි"</t>
+  </si>
+  <si>
+    <t>"@MatiBole එන්නේම නැති උනොත්."</t>
+  </si>
+  <si>
+    <t>"@AyeshaShehani බොහෝම ස්තූතියි අයේසෝ! ඉක්මනට දවසක හම්බෙමු? තිසූගෙන් කේක් ගන්නත් තියේ."</t>
+  </si>
+  <si>
+    <t>"@DraXTwitt උඹ දැන් වැඩ කරන තනේ නැති උනොත් එහා තනට පැනපං. ගොඩං වෙලාවට ඔව්වා එක වගේ 😂😂🤣"</t>
+  </si>
+  <si>
+    <t>"🍃.......... අපි ආයෙත් හමු නොවුනා නම් ඉස්සර දවසක මියගිය සෙනෙහස යලි ඉපදී මා හද හඬවන්නට අපි ආයෙත් හමු නොවුනා නම්...🍂 #සදාකාලිකනොවූලෝකේ"</t>
+  </si>
+  <si>
+    <t>"@Jude_H_Fernando @piumi_silva ආයේ ඒවා ගැන හිතලා හිත මෙව්වා කර ගන්න එපා."</t>
+  </si>
+  <si>
+    <t>"@_Thamarasa_ එල එල.. නැත්තන් අපෙ අම්මලගෙ ගමේ එන දවසක මම එනවා ඔහේ..😂😂😂"</t>
+  </si>
+  <si>
+    <t>"@Annnuza අාහ් එහෙමද.. එල.. පස්සෙ දවසක සෙට් වෙමු එහෙනම්..."</t>
+  </si>
+  <si>
+    <t>"@_ouTliER__ අගමැති උනොත් මට රස්සාවක් දෙන්න අක්කේ"</t>
+  </si>
+  <si>
+    <t>"@maalupaan බැරිම උනොත් වරෙන් මෙහෙ. ගහල කීයක් හරි හොයන් ජීවත් වෙමු. මම කීවේ ෆොටෝ ගහල."</t>
+  </si>
+  <si>
+    <t>"@FriendsGammadda ඒ makeup කරන දේවල් නෙමෙ.අනික මං makeup කරන්න දන්නේ නෑ 😂 වැඩිම උනොත් lipstick සහ eye liner පාවිච්චි කරයි 😂"</t>
+  </si>
+  <si>
+    <t>"@Jude_H_Fernando හම්මේ ඉතින් 😂👊... මේ මාසෙ ෆුල් බිසී නසියරේ.. හම්බවෙමුකො දවසක 🖤"</t>
+  </si>
+  <si>
+    <t>"@SHAN_EVO_ දවසක එන්නම් බීලා යන්න 🍻"</t>
+  </si>
+  <si>
+    <t>"@PinkySandaruwni අපි හිතලා ඒක කරලා දෙමු... අකැමැති වෙන්න දෙයක් නෑ.. අපි දෙන්නට කැමතියිනේ 😏"</t>
+  </si>
+  <si>
+    <t>"@SHAN_EVO_ @CHIRU_Vibes කෝමත් දවසක මීට් වෙමුකෝ 😊"</t>
+  </si>
+  <si>
+    <t>"@nadeerap6 තවම.නෑ ඉස්සරහට නැති උනොත් කියන්නම්කො"</t>
+  </si>
+  <si>
+    <t>"@RShashiya @PinkySandaruwni සස් පෙන් අනේ ඇන්ටිගේ යාලුවෙක් උනොත් කියල කියන්නෙ 😂"</t>
+  </si>
+  <si>
+    <t>"@PinkySandaruwni @RakzzMaduOnline මොන පෙන් උනොත්.. ???"</t>
+  </si>
+  <si>
+    <t>"අහල පහල ගෙදරකින් #රතුමකරාFM එකේ ඔටෝ ප්ලේ යන සිංදු වගේ සෙට් එකක් ඇහෙනවා.. 🤔 සැක සහිතයි.."</t>
+  </si>
+  <si>
+    <t>"@da_sukiya @imhiran99 ඔය රිප්ලයි එක මකාං යකෝ. බඩු බනිස්වෙයි. ඉංගිරිසියෙන් ප්‍රොනව්න්ස් උනාට අකුරු සිංහල උනොත් කේස්"</t>
+  </si>
+  <si>
+    <t>"මාගේ දෑස දෙස බලනු! මෙතැන් පටන් ඔබ ඇසිපිය ගහන්නෙ හිතින් හිතලා."</t>
+  </si>
+  <si>
+    <t>"අපෙ ගෙවල් පැත්ත අරාබිය වගෙ උනාට මෙ ලගදි දවසක රුවැති යුවැතියක් පැමිනියා අම්මො අම්මො"</t>
+  </si>
+  <si>
+    <t>"ජිම් යන එකට් එපා වෙලා තියෙන්නෙ කිලෝ දෙකක් වැඩි උනොත් ඊලග සතියෙ කිලෝ තුනක් අඩු වෙනවා😑"</t>
+  </si>
+  <si>
+    <t>"ලෝගන් කෝ සුඛියා කෝ අරූ කෝ මු කෝ කියලා අහන උන් තමා කවදාහරි බැන්ඳ දවසක ගෑණි කෝ කියලා හොයන්නේ 🙄"</t>
+  </si>
+  <si>
+    <t>"හොයලා හොයලා කොල්ලෙක් හොයා ගන්නම බැරි උනොත් මම හම්සව බදිනවා"</t>
+  </si>
+  <si>
+    <t>"දත් දොස්තර කෝ?? මගෙ වෙඩිමට පරක්කු වෙනවා."</t>
+  </si>
+  <si>
+    <t>"බීලා මාට්ටු උනොත් වල් අලි ගහනවා යකෝ. 😂"</t>
+  </si>
+  <si>
+    <t>"උඹල මෙහෙම සබ් ගහනවා කියලා දන්නවනම් මම දවසක් පරක්කු⁣ වෙලා ඉපදෙනවා.. - මීට චෙත්‍යා"</t>
+  </si>
+  <si>
+    <t>"@maalupaan මම සැක කලා. ඒ දරුවා මුල සිටම මං ගැන අමනාපෙන් හිටියේ. ඉතින් මමත් ඒ වගේ අය පැත්තකට කරලා නොසොයා හිටියේ. ඒකයි එක පාර මතක නැති උනේ. හැබැයි එයාගේ බුදු ෆිට් ලිස්ට් එකේ ඔයත් හිටියද? කීයටවත් වෙන්න බෑ"</t>
+  </si>
+  <si>
+    <t>"ඉරාකය, ඇෆ්ගනිස්ථානය, පකිස්ථානය, සිරියාව, ලිබියාව සහ තවත් රටවල් වල ලමයි ජනතාව මරනව live බලව් හිටපු ඔබාමා නියම පාලකයෙක්ලු.. Check out @childrenshealth’s Tweet: https://t.co/OfiBKLXBGT"</t>
+  </si>
+  <si>
+    <t>"සිංගප්පූරුව දියුණු කරපු මිනිහා වැඩ පටං ගත්තේ මෙන්න මෙහෙමයි.. ඒයා ලඟ තිබුනේ කාරණා තුනයි.. උවමනාව, කැපවීම සහ හැකියාව.. රටවල් දියුණු කරන්න දේශපාලන experience අනිවාර්ය නෑ.. #lka #GR2020 https://t.co/v9U3oyNbPs"</t>
+  </si>
+  <si>
+    <t>"ඉරාකය, ඇෆ්ගනිස්ථානය, පකිස්ථානය, සිරියාව, ලිබියාව සහ තවත් රටවල් වල ලමයි ජනතාව මරනව live බලව් හිටපු ඔබාමා නියම පාලකයෙක්ලු.. ළමයි මැරුවට මොකද නත්තලට ළමයින්ට බඩු බෙදුවනේ...🎅🎅🎅 මේව රඟපෑම් එහෙම නෙමෙයි හොඳෙ.. https://t.co/0CEV50nwAm"</t>
+  </si>
+  <si>
+    <t>"@notNaughtyE දන්නේ නෑ මෙයා. සුද්දා ගල විද්ද නිසා තමයි අපි යාන්තම් කොළඹ හරි යන්නේ. නුවර අපිට එහෙම මහලොකු දැනුමක් නැහැ. ඒකයි ඇත්ත. අනිත් රටවල් වලත් එහෙමද කියන්න එහේ යන්න තියා ඉන්ටර්නෙට් එකේ සර්ච් කරලා ඒ දේවල් බලන්නවත් අපිට ඉංග්‍රීසි දන්නේ නෑ 😢"</t>
+  </si>
+  <si>
+    <t>"&amp;lt;3 මගේ ආදරේ තවමත් ඒ වගේ සොදුරු කතාවක් වගේ නුබේ හීනයේ දැවටී එදා වගේ ඉන්න ආසයි තවමත් හිතේ දවසක නුබ හා මේ ගී පද ගැලපු තනුවක් වාගේ නුබ මට මියුරු එන මග සරසා නුබ යනවිට තනිවූ දවසක් ඒවිද ආයෙත් නුබ මට හිමි වූ.. &amp;lt;3 https://t.co/7OPJnK4RSs"</t>
+  </si>
+  <si>
+    <t>"@Nimal15700736 @cleanpoltics @NimaliWijesuri3 @ApiWenuwen @JMLPBandara @GayaniGunaseke2 @nnalani1231 @ranjanieguruge @CBSL @RW_UNP @HarshadeSilvaMP @EranWick @MangalaLK @MaithripalaS @Senaratne77 @Neetwit @PresRajapaksa @ParliamentLK @randheeraM @nilanp @astroanu @hithuwakkari89 @galpathatlr @KalyanaMithraya @medaperadiga @AsIFxOubyozDmOY @ra5tha @Sudumameduvada @WasthiOfficial @DooWeere @udanaekanayake @Dilanka_ss @hesha_UNP01 @PiyumiShashi @Media_NR @tmfallen @Ru_Weerasuriya @vishiru @LUshimarie @paranawithana @JosephMorgan @amalab @mihywun @Aqua097 @hima_flake @LankanJokes @Yawathashi @ManoGanesan @PodujanaParty මේ ගිවිසුම හරහා අපේ රටේ සේවා ටික සිංගප්පූරුවට පමණක් නොවෙයි පාවලා දීලා තිබෙන්නේ. ඉන්දියාව, චීනය, මැලේසියාව කියන රටවල් හමුවේ පාවලා දීලා තිබෙනවා. 1815 අපේ රට සුද්දාට විතරයි යටත් වුණේ. නමුත් ලෝකයේ සියලු රටවල් හමුවේ අපිව පාවා දීලා ඉවරයි මේ https://t.co/imfO4FngUd https://t.co/F4qhD3dpJK"</t>
+  </si>
+  <si>
+    <t>"වැරදි දැක්කත් ඒවා ප්‍රසිද්ධ කරලා තමන්ගෙ ආගම ගැන තියන වටිනාකම,බක්තිය අන්ආගමිකයන් ඉස්සරා නැති කර ගන්නෙ නෑ.අපිට හිතන්න සෑහෙන්න දේවල් තියෙනවා රැඩිකල් විදිහට හිතලා ටෑටු එකක් සාධාරණීකරනය කරන්න කලින්."</t>
+  </si>
+  <si>
+    <t>"එන්න දවසක. ඇවිත් මගෙ හදවතත් මෙගා පික්සල් බිලියන විසිහතරදාකට කඩල සූම් කරල බලන්න ඒ හැම කොන්ටම් අංශුවකම ආදරේ තියේවි ඔයාගෙ නමින් ලියවිලා හැමදාටම .... ❤️ යෝ..යෝ... #බොබී"</t>
+  </si>
+  <si>
+    <t>"ඔයාටත් ඉන්නවද? පාරෙ යද්දි අඳුරන අය ඉස්සරහට එද්දි අත අතාරින ඔයා එයාගෙ යාලුවෙක් විතරයි කියලා හැමෝටම කියලා තියන හැම තිස්සෙම නිදහසට කාරණා කිය කිය කාර්‍යබහුල බව අඟවන, ඒත් online ඉන්න හැම දේටම බොරුවට සැක කරන, හේතු හදාගෙන තරහ වෙන .............කෙනෙක්??? 😔😔"</t>
+  </si>
+  <si>
+    <t>"මේම පැටලැවිල්ලක් උනොත් තමා අපිට කෝල් එන්නේ.. නැත්තම් කොල් කරන්නේ අර dialog එකෙන් බූට් සින්දු call a tune දාගන්න කියන කෝල් එක තමා..😂😂 https://t.co/8ctmWnrSGc"</t>
+  </si>
+  <si>
+    <t>"අතීතයට ගිහින් දේවල් වෙනස් කරනවා කියන මිත්‍යාව මිත්‍යාවක් ලෙසටම හැමදාම තියෙනවනම් හොඳයි. අනාගතයක් කියලා දෙයක් නැත්තටම නැති වෙන්න පුලුවන් එහෙම උනොත්."</t>
+  </si>
+  <si>
+    <t>"ගෙදරින් පිට, බෝඩිං වල ඉන්නකොට ගෙදර වෙන කිසිම අවුලක් තාත්තා මට කියන්නෙ නෑ. වෙන අයට කියන්න දෙන්නෙත් නෑ. අම්මා මොකක් හරි කියන්න යනකොට පැනලා ඒක නවත්තනවා. ඒ මම ඒවා හිතට අරන් ඔළුවට වදයක් කරගනී කියලා හිතලා ලු. තාත්තලාගෙ ආදරේ හරි වෙනස්. ගැඹුරුයි. සමහරවිට තේරුම්ගන්නත් අමාරුයි. 😌❤️"</t>
+  </si>
+  <si>
+    <t>"මට ජිවිතේ කවදාකවත් නුවර යන්න හේතුවක් ඕනි වුණේ නෑ.. දළදා මාලිගාව ඉස්සරහින් වැව දිගේ යද්දී , මාලිගාවෙන් එන සුවද , ඒ මගුල්බෙර වාදනය නිසා හිතට පුදුම සැහැල්ලුවක් දැනෙන්නේ.. මේ අවුරුදු ගානටම සෙරෙප්පු දෙක හිතලා ගලවනවා නෙවෙයි ... කකුල් වලින් සෙරෙප්පු දෙක ගැලවෙනවා ශ්‍රී දන්ත ධාතුව 👇"</t>
+  </si>
+  <si>
+    <t>"‌සමහර එවුන් මේකට එන්නෙම කෙනෙක් කරන වැඩේ නතර කරලා මොකක් හරි පොර ටෝක් එකක් දීලා යන්න. උන් කරන්නෙත් නෑ, කරන එවුන්ට කරන්න දෙන්නෙත් නෑ. ඕකුන් තමයි කවදාහරි බැන්ද දවසක පලමු රාත්‍රීයේ යාලුවන්ට කෝල් කර කර " ඒ මචන් මොකෝ බං මං දැන් කරන්න ඕන, නිදාගත්තට කමක් නැද්ද " කිය කිය ඇඩ්වයිස් ගන්නේ. 😅"</t>
+  </si>
+  <si>
+    <t>"@DeV_DaZ අපාරාදෙ කියන්නෙ බැ මෙකෙ ඉන්න මිනිසුන් කවද හරි දවසක් ඔය administer role එකක්.කරොත් තමන්ගේ service ගන්න පුද්ගලයෙක් අසාධාරණයක් උනොත් පිලිසරණ ක් නැ මොලෙ පරිණත වෙලා.නැ එකතාමා අවුල"</t>
+  </si>
+  <si>
+    <t>"දුම්රියේ යන කට්ටියගෙන් මෙච්චර කල් කිසි උදව්වක් ඉල්ලලා නෑ මං...අද පොඩි උදව්වක් ඉල්ලන්න කල්පනා කරා... https://t.co/AQkH2cpR8y Train ඇප් එකට Vote කරලා උදව්වක් කරන්න...හැමදාම පරක්කු වෙන කෝච්චිය ගැන Update ගන්නවා වගේම සේවය ලබාගත්... https://t.co/8NiYoxy4sY"</t>
+  </si>
+  <si>
+    <t>"@ranukad යකෝ කවුරු හරි මුල්වෙලා එහෙම දෙයක් කරන නිසයි එන්න බැරි වුනත් මුන්ටික ආතල් එකක් ගන්නවා නේද කියලා හිතලා හරි සතුටුවෙන්නේ..! අහක ඉන්න වේස නරි එක එක ඒවා කිව්වා කියලා, උඹලා කරන වැඩ නවත්තන්න හිතනවා නං, මට කියන්න තියෙන්නේ අනේ මංදා කියලා තමා රනුක.! 😑"</t>
+  </si>
+  <si>
+    <t>"හිතෙන විකාර ට්වීට් කරලා හැමදාම දැම්මා. ඒකෙ චුට්ටං හරි ආර්ට් එකක් දැකලා #ජොබ්එකගාවගමු කියලා හිතලා @moogater අක්කා ලියන්න උදව්කරා. ඇයි අනිත් අයටත් ඒ වගේ හොඳ විදිහට අනිත් අයට උදව්කරන්න බැරි?"</t>
+  </si>
+  <si>
+    <t>"එයා කිවුවා කැටයක් අරගෙන හැමදාම ඒකට රුපියක් දහය ගානේ හරි.. ඊට වැඩියෙන් හරි දාන්න කියලා. හොද දෙයක් වෙනුවෙන් කිවුවා.දවසක ආයෙත් මගේ ලගට එනවා කිවුවා හේතුවත් අරගෙනම. මොකක්ද ඒ මාරම පස්නයක් ඒක..... 🧐🧐🧐🧐🧐🧐🧐🧐 #දැවෙනප්‍රශ්න"</t>
+  </si>
+  <si>
+    <t>"Naththal Awa - Latha Walpola and Eranga Lanka නත්තල් ආවා ආවා ආවා ජේසු බිලිඳු ආවා උඳුවප් මාසේ සීතල දවසක මැදියම් රෑ යාමේ බෙත්ලෙහෙමේ පුංචි ගවලෙනේ ජේසු උපත වූයේ සාමයේ අරුණලු දසත පැතිර ගියේ නත්තලේ අපි... https://t.co/cOu1xPZhFm"</t>
+  </si>
+  <si>
+    <t>"ලෝගා දාපු එක ඩුප්ලිකේට් ගහන්නත් හිතලා ආයේ අතෑරියා. සයිබර් බුලින් කරලා රස්සාව නැති කරගන්න බෑ. ලෝගව රිපෝර්ට් කලා හේට් ස්පීච් කියලා. වෙලාවට ඌ රිපෝර්ට් කරන විදිහ කලින් කියලා තිබුනේ 😂"</t>
+  </si>
+  <si>
+    <t>"එතකොට බැරිවෙලාවත් ඒකාබද්ධෙන් ආන්ඩුව පිහිටවලා තිබිලා ඒකට unp එකෙන් කවුරු හරි පැන්නොත් ඇමතිකම් දෙනවා. හැබැයි, Unp එකෙන් ආන්ඩු පිහිටවලා ඒකට ඒකාබද්දේ හෝ නිදහස් පක්ශේ කවුරු හරි unp එක එක්කලා එක්කහු උනොත් එතකොට ඇමතිකම් නෑ. මෛත්‍රිපාලගෙත් තියෙන්නේ ටෞකණ තියරි බොල..! 🤭🤔"</t>
+  </si>
+  <si>
+    <t>"@sanathk53122963 ගල් ගොඩ උඩ ඉන්න ඇච්චා 😂👋"</t>
+  </si>
+  <si>
+    <t>"*සාරංශය....* ***'අායුෂ කෙටියි'*** වැඩිය 'උඩ පනින' 'කෑැැ....ගහන' 'දගලන' කාට කාටත්.....ඔන්න කිව්වා🧐🤔🧐 https://t.co/FISpuezJCI"</t>
+  </si>
+  <si>
+    <t>"පාරෙ යන මිනිස්සු මං දිහා බල බල යනව..මොකක් හරි අවුලක්වත්ද මගෙ..😲😧"</t>
+  </si>
+  <si>
+    <t>"@ayajnaz උඩ යන්න එපා😏"</t>
+  </si>
+  <si>
+    <t>"@NandiyaLive අපි හිටපු විදිහේ මොකක් මතක් වෙන්නද බං !! එදත් පිස්සු කෙලිය අදත් එහෙම තමා 😉උබ දැන් ඉන්න විදිහ හොදයි !!"</t>
+  </si>
+  <si>
+    <t>"@Sansajran ඒ කියන්නෙ ඕන කෙනෙක් සදුන් ගැන දන්නව😂"</t>
+  </si>
+  <si>
+    <t>"@KawdaBoy @piumi_silva @itzJambole මම ඉතිං උඩ abroad ඉන්නේ 😂"</t>
+  </si>
+  <si>
+    <t>"ඔය මොකක් හරි එකක් දාල...2009 කියල කියන්න.😁🙏 https://t.co/Gee0mzDjo6"</t>
+  </si>
+  <si>
+    <t>"@FriendsGammadda අනේ එතකොට නම් උඩ බිම ඉන්න බැහැ රශ්නය නිසා.තව ජර්සී දැම්මොත් හොදට තියේ...😂😂"</t>
+  </si>
+  <si>
+    <t>"ඕනෑවට වඩා උඩ තැබීමෙන් වලකින්න. බිමට බහින්නට බැරිවිය හැක."</t>
+  </si>
+  <si>
+    <t>"@BasnayakageGopi මොකක් 🤔🤔😂"</t>
+  </si>
+  <si>
+    <t>"@ItzmeNeepi මේසෙ උඩ තියන පෝන් එක දැක්ක 😒😒😒😒"</t>
+  </si>
+  <si>
+    <t>"ඇච්චා කලේ ඉඳලම ගල් උඩ තමා 😂👋😂👋 https://t.co/7wlqNZ4orQ"</t>
+  </si>
+  <si>
+    <t>"@pasiya14 දන්නව😂😂"</t>
+  </si>
+  <si>
+    <t>"@maalupaan එයාට මොකක් දැම්මත් ලයික්ස් රිප්ලයිස්. ඉරිසියයිත් එක්ක. 😩"</t>
+  </si>
+  <si>
+    <t>"@amalskr ඔව්.නැත්නම් ඔවුන් උඩ යනවා තවත්."</t>
+  </si>
+  <si>
+    <t>"@Chami08416797 බංගි උඩ බලන් බුරනවා 😁 ඒක ඊට වඩා වදේ එතකොට"</t>
   </si>
 </sst>
 </file>
@@ -1772,7 +2069,7 @@
   <dimension ref="A1:D914"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A324" workbookViewId="0">
-      <selection activeCell="B329" sqref="B329"/>
+      <selection activeCell="B333" sqref="B333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5144,509 +5441,913 @@
       </c>
     </row>
     <row r="331" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B331" s="11"/>
-      <c r="C331" s="12"/>
-      <c r="D331" s="11"/>
-    </row>
-    <row r="332" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B332" s="11"/>
-      <c r="C332" s="12"/>
-      <c r="D332" s="11"/>
-    </row>
-    <row r="333" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B333" s="11"/>
-      <c r="C333" s="12"/>
-      <c r="D333" s="11"/>
+      <c r="B331" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="C331"/>
+      <c r="D331" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="332" spans="2:4" ht="60.75" thickBot="1">
+      <c r="B332" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="C332"/>
+      <c r="D332" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="333" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B333" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="C333"/>
+      <c r="D333" s="11" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="334" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B334" s="11"/>
-      <c r="C334" s="12"/>
-      <c r="D334" s="11"/>
-    </row>
-    <row r="335" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B335" s="11"/>
-      <c r="C335" s="12"/>
-      <c r="D335" s="11"/>
-    </row>
-    <row r="336" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B336" s="11"/>
-      <c r="C336" s="12"/>
-      <c r="D336" s="11"/>
-    </row>
-    <row r="337" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B337" s="11"/>
-      <c r="C337" s="12"/>
-      <c r="D337" s="11"/>
-    </row>
-    <row r="338" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B338" s="11"/>
-      <c r="C338" s="12"/>
-      <c r="D338" s="11"/>
-    </row>
-    <row r="339" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B339" s="11"/>
-      <c r="C339" s="12"/>
-      <c r="D339" s="11"/>
-    </row>
-    <row r="340" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B340" s="11"/>
-      <c r="C340" s="12"/>
-      <c r="D340" s="11"/>
-    </row>
-    <row r="341" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B341" s="11"/>
-      <c r="C341" s="12"/>
-      <c r="D341" s="11"/>
-    </row>
-    <row r="342" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B342" s="11"/>
-      <c r="C342" s="12"/>
-      <c r="D342" s="11"/>
-    </row>
-    <row r="343" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B343" s="11"/>
-      <c r="C343" s="12"/>
-      <c r="D343" s="11"/>
-    </row>
-    <row r="344" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B344" s="11"/>
-      <c r="C344" s="12"/>
-      <c r="D344" s="11"/>
-    </row>
-    <row r="345" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B345" s="11"/>
-      <c r="C345" s="12"/>
-      <c r="D345" s="11"/>
-    </row>
-    <row r="346" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B346" s="11"/>
-      <c r="C346" s="12"/>
-      <c r="D346" s="11"/>
-    </row>
-    <row r="347" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B347" s="11"/>
-      <c r="C347" s="12"/>
-      <c r="D347" s="11"/>
-    </row>
-    <row r="348" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B348" s="11"/>
-      <c r="C348" s="12"/>
-      <c r="D348" s="11"/>
-    </row>
-    <row r="349" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B349" s="11"/>
-      <c r="C349" s="12"/>
-      <c r="D349" s="11"/>
-    </row>
-    <row r="350" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B350" s="11"/>
-      <c r="C350" s="12"/>
-      <c r="D350" s="11"/>
-    </row>
-    <row r="351" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B351" s="11"/>
-      <c r="C351" s="12"/>
-      <c r="D351" s="11"/>
-    </row>
-    <row r="352" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B352" s="11"/>
-      <c r="C352" s="12"/>
-      <c r="D352" s="11"/>
-    </row>
-    <row r="353" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B353" s="11"/>
-      <c r="C353" s="12"/>
-      <c r="D353" s="11"/>
-    </row>
-    <row r="354" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B354" s="11"/>
-      <c r="C354" s="12"/>
-      <c r="D354" s="11"/>
-    </row>
-    <row r="355" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B355" s="11"/>
-      <c r="C355" s="12"/>
-      <c r="D355" s="11"/>
-    </row>
-    <row r="356" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B356" s="11"/>
-      <c r="C356" s="12"/>
-      <c r="D356" s="11"/>
-    </row>
-    <row r="357" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B357" s="11"/>
-      <c r="C357" s="12"/>
-      <c r="D357" s="11"/>
-    </row>
-    <row r="358" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B358" s="11"/>
-      <c r="C358" s="12"/>
-      <c r="D358" s="11"/>
-    </row>
-    <row r="359" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B359" s="11"/>
-      <c r="C359" s="12"/>
-      <c r="D359" s="11"/>
-    </row>
-    <row r="360" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B360" s="11"/>
-      <c r="C360" s="12"/>
-      <c r="D360" s="11"/>
+      <c r="B334" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="C334"/>
+      <c r="D334" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="335" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B335" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="C335"/>
+      <c r="D335" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="336" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B336" s="11" t="s">
+        <v>444</v>
+      </c>
+      <c r="C336"/>
+      <c r="D336" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="337" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B337" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="C337"/>
+      <c r="D337" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="338" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B338" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="C338"/>
+      <c r="D338" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="339" spans="2:4" ht="60.75" thickBot="1">
+      <c r="B339" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="C339"/>
+      <c r="D339" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="340" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B340" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="C340"/>
+      <c r="D340" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="341" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B341" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="C341"/>
+      <c r="D341" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="342" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B342" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="C342"/>
+      <c r="D342" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="343" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B343" s="11" t="s">
+        <v>451</v>
+      </c>
+      <c r="C343"/>
+      <c r="D343" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="344" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B344" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="C344"/>
+      <c r="D344" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="345" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B345" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="C345"/>
+      <c r="D345" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="346" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B346" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="C346"/>
+      <c r="D346" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="347" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B347" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="C347"/>
+      <c r="D347" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="348" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B348" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="C348"/>
+      <c r="D348" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="349" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B349" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="C349"/>
+      <c r="D349" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="350" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B350" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="C350"/>
+      <c r="D350" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="351" spans="2:4" ht="60.75" thickBot="1">
+      <c r="B351" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="C351"/>
+      <c r="D351" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="352" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B352" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="C352"/>
+      <c r="D352" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="353" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B353" s="11" t="s">
+        <v>461</v>
+      </c>
+      <c r="C353"/>
+      <c r="D353" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="354" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B354" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="C354"/>
+      <c r="D354" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="355" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B355" s="11" t="s">
+        <v>463</v>
+      </c>
+      <c r="C355"/>
+      <c r="D355" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="356" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B356" s="11" t="s">
+        <v>464</v>
+      </c>
+      <c r="C356"/>
+      <c r="D356" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="357" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B357" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="C357"/>
+      <c r="D357" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="358" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B358" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="C358"/>
+      <c r="D358" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="359" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B359" s="11" t="s">
+        <v>467</v>
+      </c>
+      <c r="C359"/>
+      <c r="D359" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="360" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B360" s="11" t="s">
+        <v>468</v>
+      </c>
+      <c r="C360"/>
+      <c r="D360" s="11" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="361" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B361" s="11"/>
-      <c r="C361" s="12"/>
-      <c r="D361" s="11"/>
-    </row>
-    <row r="362" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B362" s="11"/>
-      <c r="C362" s="12"/>
-      <c r="D362" s="11"/>
+      <c r="B361" s="11" t="s">
+        <v>469</v>
+      </c>
+      <c r="C361"/>
+      <c r="D361" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="362" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B362" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="C362"/>
+      <c r="D362" s="11" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="363" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B363" s="11"/>
-      <c r="C363" s="12"/>
-      <c r="D363" s="11"/>
-    </row>
-    <row r="364" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B364" s="11"/>
-      <c r="C364" s="12"/>
-      <c r="D364" s="11"/>
-    </row>
-    <row r="365" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B365" s="11"/>
-      <c r="C365" s="12"/>
-      <c r="D365" s="11"/>
-    </row>
-    <row r="366" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B366" s="11"/>
-      <c r="C366" s="12"/>
-      <c r="D366" s="11"/>
-    </row>
-    <row r="367" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B367" s="11"/>
-      <c r="C367" s="12"/>
-      <c r="D367" s="11"/>
-    </row>
-    <row r="368" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B368" s="11"/>
-      <c r="C368" s="12"/>
-      <c r="D368" s="11"/>
-    </row>
-    <row r="369" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B369" s="11"/>
-      <c r="C369" s="12"/>
-      <c r="D369" s="11"/>
-    </row>
-    <row r="370" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B370" s="11"/>
-      <c r="C370" s="12"/>
-      <c r="D370" s="11"/>
-    </row>
-    <row r="371" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B371" s="11"/>
-      <c r="C371" s="12"/>
-      <c r="D371" s="11"/>
-    </row>
-    <row r="372" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B372" s="11"/>
-      <c r="C372" s="12"/>
-      <c r="D372" s="11"/>
-    </row>
-    <row r="373" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B373" s="11"/>
-      <c r="C373" s="12"/>
-      <c r="D373" s="11"/>
+      <c r="B363" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="C363"/>
+      <c r="D363" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="364" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B364" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="C364"/>
+      <c r="D364" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="365" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B365" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="C365"/>
+      <c r="D365" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="366" spans="2:4" ht="60.75" thickBot="1">
+      <c r="B366" s="11" t="s">
+        <v>474</v>
+      </c>
+      <c r="C366"/>
+      <c r="D366" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="367" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B367" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="C367"/>
+      <c r="D367" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="368" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B368" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="C368"/>
+      <c r="D368" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="369" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B369" s="11" t="s">
+        <v>477</v>
+      </c>
+      <c r="C369"/>
+      <c r="D369" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="370" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B370" s="11" t="s">
+        <v>478</v>
+      </c>
+      <c r="C370"/>
+      <c r="D370" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="371" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B371" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="C371"/>
+      <c r="D371" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="372" spans="2:4" ht="60.75" thickBot="1">
+      <c r="B372" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="C372"/>
+      <c r="D372" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="373" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B373" s="11" t="s">
+        <v>481</v>
+      </c>
+      <c r="C373"/>
+      <c r="D373" s="11" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="374" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B374" s="11"/>
-      <c r="C374" s="12"/>
-      <c r="D374" s="11"/>
-    </row>
-    <row r="375" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B375" s="11"/>
-      <c r="C375" s="12"/>
-      <c r="D375" s="11"/>
-    </row>
-    <row r="376" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B376" s="11"/>
-      <c r="C376" s="12"/>
-      <c r="D376" s="11"/>
-    </row>
-    <row r="377" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B377" s="11"/>
-      <c r="C377" s="12"/>
-      <c r="D377" s="11"/>
-    </row>
-    <row r="378" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B378" s="11"/>
-      <c r="C378" s="12"/>
-      <c r="D378" s="11"/>
-    </row>
-    <row r="379" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B379" s="11"/>
-      <c r="C379" s="12"/>
-      <c r="D379" s="11"/>
-    </row>
-    <row r="380" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B380" s="11"/>
-      <c r="C380" s="12"/>
-      <c r="D380" s="11"/>
-    </row>
-    <row r="381" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B381" s="11"/>
-      <c r="C381" s="12"/>
-      <c r="D381" s="11"/>
-    </row>
-    <row r="382" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B382" s="11"/>
-      <c r="C382" s="12"/>
-      <c r="D382" s="11"/>
-    </row>
-    <row r="383" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B383" s="11"/>
-      <c r="C383" s="12"/>
-      <c r="D383" s="11"/>
-    </row>
-    <row r="384" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B384" s="11"/>
-      <c r="C384" s="12"/>
-      <c r="D384" s="11"/>
-    </row>
-    <row r="385" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B385" s="11"/>
-      <c r="C385" s="12"/>
-      <c r="D385" s="11"/>
-    </row>
-    <row r="386" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B386" s="11"/>
-      <c r="C386" s="12"/>
-      <c r="D386" s="11"/>
-    </row>
-    <row r="387" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B387" s="11"/>
-      <c r="C387" s="12"/>
-      <c r="D387" s="11"/>
-    </row>
-    <row r="388" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B388" s="11"/>
-      <c r="C388" s="12"/>
-      <c r="D388" s="11"/>
+      <c r="B374" s="11" t="s">
+        <v>482</v>
+      </c>
+      <c r="C374"/>
+      <c r="D374" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="375" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B375" s="11" t="s">
+        <v>483</v>
+      </c>
+      <c r="C375"/>
+      <c r="D375" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="376" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B376" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="C376"/>
+      <c r="D376" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="377" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B377" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="C377"/>
+      <c r="D377" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="378" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B378" s="11" t="s">
+        <v>486</v>
+      </c>
+      <c r="C378"/>
+      <c r="D378" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="379" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B379" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="C379"/>
+      <c r="D379" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="380" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B380" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="C380"/>
+      <c r="D380" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="381" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B381" s="11" t="s">
+        <v>489</v>
+      </c>
+      <c r="C381"/>
+      <c r="D381" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="382" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B382" s="11" t="s">
+        <v>490</v>
+      </c>
+      <c r="C382"/>
+      <c r="D382" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="383" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B383" s="11" t="s">
+        <v>491</v>
+      </c>
+      <c r="C383"/>
+      <c r="D383" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="384" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B384" s="11" t="s">
+        <v>492</v>
+      </c>
+      <c r="C384"/>
+      <c r="D384" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="385" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B385" s="11" t="s">
+        <v>493</v>
+      </c>
+      <c r="C385"/>
+      <c r="D385" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="386" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B386" s="11" t="s">
+        <v>494</v>
+      </c>
+      <c r="C386"/>
+      <c r="D386" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="387" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B387" s="11" t="s">
+        <v>494</v>
+      </c>
+      <c r="C387"/>
+      <c r="D387" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="388" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B388" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="C388"/>
+      <c r="D388" s="11" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="389" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B389" s="11"/>
-      <c r="C389" s="12"/>
-      <c r="D389" s="11"/>
-    </row>
-    <row r="390" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B390" s="11"/>
-      <c r="C390" s="12"/>
-      <c r="D390" s="11"/>
-    </row>
-    <row r="391" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B391" s="11"/>
-      <c r="C391" s="12"/>
-      <c r="D391" s="11"/>
-    </row>
-    <row r="392" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B392" s="11"/>
-      <c r="C392" s="12"/>
-      <c r="D392" s="11"/>
-    </row>
-    <row r="393" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B393" s="11"/>
-      <c r="C393" s="12"/>
-      <c r="D393" s="11"/>
-    </row>
-    <row r="394" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B394" s="11"/>
-      <c r="C394" s="12"/>
-      <c r="D394" s="11"/>
-    </row>
-    <row r="395" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B395" s="11"/>
-      <c r="C395" s="12"/>
-      <c r="D395" s="11"/>
-    </row>
-    <row r="396" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B396" s="11"/>
-      <c r="C396" s="12"/>
-      <c r="D396" s="11"/>
-    </row>
-    <row r="397" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B397" s="11"/>
-      <c r="C397" s="12"/>
-      <c r="D397" s="11"/>
-    </row>
-    <row r="398" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B398" s="11"/>
-      <c r="C398" s="12"/>
-      <c r="D398" s="11"/>
-    </row>
-    <row r="399" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B399" s="11"/>
-      <c r="C399" s="12"/>
-      <c r="D399" s="11"/>
-    </row>
-    <row r="400" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B400" s="11"/>
-      <c r="C400" s="12"/>
-      <c r="D400" s="11"/>
-    </row>
-    <row r="401" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B401" s="11"/>
-      <c r="C401" s="12"/>
-      <c r="D401" s="11"/>
-    </row>
-    <row r="402" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B402" s="11"/>
-      <c r="C402" s="12"/>
-      <c r="D402" s="11"/>
-    </row>
-    <row r="403" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B403" s="11"/>
-      <c r="C403" s="12"/>
-      <c r="D403" s="11"/>
-    </row>
-    <row r="404" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B404" s="11"/>
-      <c r="C404" s="12"/>
-      <c r="D404" s="11"/>
-    </row>
-    <row r="405" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B405" s="11"/>
-      <c r="C405" s="12"/>
-      <c r="D405" s="11"/>
-    </row>
-    <row r="406" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B406" s="11"/>
-      <c r="C406" s="12"/>
-      <c r="D406" s="11"/>
-    </row>
-    <row r="407" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B407" s="11"/>
-      <c r="C407" s="12"/>
-      <c r="D407" s="11"/>
-    </row>
-    <row r="408" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B408" s="11"/>
-      <c r="C408" s="12"/>
-      <c r="D408" s="11"/>
-    </row>
-    <row r="409" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B409" s="11"/>
-      <c r="C409" s="12"/>
-      <c r="D409" s="11"/>
-    </row>
-    <row r="410" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B410" s="11"/>
-      <c r="C410" s="12"/>
-      <c r="D410" s="11"/>
-    </row>
-    <row r="411" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B411" s="11"/>
-      <c r="C411" s="12"/>
-      <c r="D411" s="11"/>
-    </row>
-    <row r="412" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B412" s="11"/>
-      <c r="C412" s="12"/>
-      <c r="D412" s="11"/>
-    </row>
-    <row r="413" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B413" s="11"/>
-      <c r="C413" s="12"/>
-      <c r="D413" s="11"/>
-    </row>
-    <row r="414" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B414" s="11"/>
-      <c r="C414" s="12"/>
-      <c r="D414" s="11"/>
-    </row>
-    <row r="415" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B415" s="11"/>
-      <c r="C415" s="12"/>
-      <c r="D415" s="11"/>
-    </row>
-    <row r="416" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B416" s="11"/>
-      <c r="C416" s="12"/>
-      <c r="D416" s="11"/>
-    </row>
-    <row r="417" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B417" s="11"/>
-      <c r="C417" s="12"/>
-      <c r="D417" s="11"/>
+      <c r="B389" s="11" t="s">
+        <v>496</v>
+      </c>
+      <c r="C389"/>
+      <c r="D389" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="390" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B390" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="C390"/>
+      <c r="D390" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="391" spans="2:4" ht="90.75" thickBot="1">
+      <c r="B391" s="11" t="s">
+        <v>498</v>
+      </c>
+      <c r="C391"/>
+      <c r="D391" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="392" spans="2:4" ht="75.75" thickBot="1">
+      <c r="B392" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="C392"/>
+      <c r="D392" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="393" spans="2:4" ht="90.75" thickBot="1">
+      <c r="B393" s="11" t="s">
+        <v>500</v>
+      </c>
+      <c r="C393"/>
+      <c r="D393" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="394" spans="2:4" ht="90.75" thickBot="1">
+      <c r="B394" s="11" t="s">
+        <v>501</v>
+      </c>
+      <c r="C394"/>
+      <c r="D394" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="395" spans="2:4" ht="105.75" thickBot="1">
+      <c r="B395" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="C395"/>
+      <c r="D395" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="396" spans="2:4" ht="90.75" thickBot="1">
+      <c r="B396" s="11" t="s">
+        <v>503</v>
+      </c>
+      <c r="C396"/>
+      <c r="D396" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="397" spans="2:4" ht="345.75" thickBot="1">
+      <c r="B397" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="C397"/>
+      <c r="D397" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="398" spans="2:4" ht="90.75" thickBot="1">
+      <c r="B398" s="11" t="s">
+        <v>505</v>
+      </c>
+      <c r="C398"/>
+      <c r="D398" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="399" spans="2:4" ht="75.75" thickBot="1">
+      <c r="B399" s="11" t="s">
+        <v>506</v>
+      </c>
+      <c r="C399"/>
+      <c r="D399" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="400" spans="2:4" ht="105.75" thickBot="1">
+      <c r="B400" s="11" t="s">
+        <v>507</v>
+      </c>
+      <c r="C400"/>
+      <c r="D400" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="401" spans="2:4" ht="60.75" thickBot="1">
+      <c r="B401" s="11" t="s">
+        <v>508</v>
+      </c>
+      <c r="C401"/>
+      <c r="D401" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="402" spans="2:4" ht="60.75" thickBot="1">
+      <c r="B402" s="11" t="s">
+        <v>509</v>
+      </c>
+      <c r="C402"/>
+      <c r="D402" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="403" spans="2:4" ht="120.75" thickBot="1">
+      <c r="B403" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="C403"/>
+      <c r="D403" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="404" spans="2:4" ht="105.75" thickBot="1">
+      <c r="B404" s="11" t="s">
+        <v>511</v>
+      </c>
+      <c r="C404"/>
+      <c r="D404" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="405" spans="2:4" ht="120.75" thickBot="1">
+      <c r="B405" s="11" t="s">
+        <v>512</v>
+      </c>
+      <c r="C405"/>
+      <c r="D405" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="406" spans="2:4" ht="75.75" thickBot="1">
+      <c r="B406" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="C406"/>
+      <c r="D406" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="407" spans="2:4" ht="105.75" thickBot="1">
+      <c r="B407" s="11" t="s">
+        <v>514</v>
+      </c>
+      <c r="C407"/>
+      <c r="D407" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="408" spans="2:4" ht="105.75" thickBot="1">
+      <c r="B408" s="11" t="s">
+        <v>515</v>
+      </c>
+      <c r="C408"/>
+      <c r="D408" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="409" spans="2:4" ht="75.75" thickBot="1">
+      <c r="B409" s="11" t="s">
+        <v>516</v>
+      </c>
+      <c r="C409"/>
+      <c r="D409" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="410" spans="2:4" ht="90.75" thickBot="1">
+      <c r="B410" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="C410"/>
+      <c r="D410" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="411" spans="2:4" ht="90.75" thickBot="1">
+      <c r="B411" s="11" t="s">
+        <v>518</v>
+      </c>
+      <c r="C411"/>
+      <c r="D411" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="412" spans="2:4" ht="75.75" thickBot="1">
+      <c r="B412" s="11" t="s">
+        <v>519</v>
+      </c>
+      <c r="C412"/>
+      <c r="D412" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="413" spans="2:4" ht="75.75" thickBot="1">
+      <c r="B413" s="11" t="s">
+        <v>519</v>
+      </c>
+      <c r="C413"/>
+      <c r="D413" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="414" spans="2:4" ht="120.75" thickBot="1">
+      <c r="B414" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="C414"/>
+      <c r="D414" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="415" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B415" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="C415"/>
+      <c r="D415" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="416" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B416" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="C416"/>
+      <c r="D416" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="417" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B417" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="C417"/>
+      <c r="D417" s="11" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="418" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B418" s="11"/>
-      <c r="C418" s="12"/>
-      <c r="D418" s="11"/>
-    </row>
-    <row r="419" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B419" s="11"/>
-      <c r="C419" s="12"/>
-      <c r="D419" s="11"/>
-    </row>
-    <row r="420" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B420" s="11"/>
-      <c r="C420" s="12"/>
-      <c r="D420" s="11"/>
-    </row>
-    <row r="421" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B421" s="11"/>
-      <c r="C421" s="12"/>
-      <c r="D421" s="11"/>
-    </row>
-    <row r="422" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B422" s="11"/>
-      <c r="C422" s="12"/>
-      <c r="D422" s="11"/>
-    </row>
-    <row r="423" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B423" s="11"/>
-      <c r="C423" s="12"/>
-      <c r="D423" s="11"/>
-    </row>
-    <row r="424" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B424" s="11"/>
-      <c r="C424" s="12"/>
-      <c r="D424" s="11"/>
+      <c r="B418" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="C418"/>
+      <c r="D418" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="419" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B419" s="11" t="s">
+        <v>525</v>
+      </c>
+      <c r="C419"/>
+      <c r="D419" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="420" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B420" s="11" t="s">
+        <v>526</v>
+      </c>
+      <c r="C420"/>
+      <c r="D420" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="421" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B421" s="11" t="s">
+        <v>527</v>
+      </c>
+      <c r="C421"/>
+      <c r="D421" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="422" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B422" s="11" t="s">
+        <v>528</v>
+      </c>
+      <c r="C422"/>
+      <c r="D422" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="423" spans="2:4" ht="45.75" thickBot="1">
+      <c r="B423" s="11" t="s">
+        <v>529</v>
+      </c>
+      <c r="C423"/>
+      <c r="D423" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="424" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B424" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="C424"/>
+      <c r="D424" s="11" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="425" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B425" s="11"/>
-      <c r="C425" s="12"/>
-      <c r="D425" s="11"/>
-    </row>
-    <row r="426" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B426" s="11"/>
-      <c r="C426" s="12"/>
-      <c r="D426" s="11"/>
-    </row>
-    <row r="427" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B427" s="11"/>
-      <c r="C427" s="12"/>
-      <c r="D427" s="11"/>
+      <c r="B425" s="11" t="s">
+        <v>531</v>
+      </c>
+      <c r="C425"/>
+      <c r="D425" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="426" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B426" s="11" t="s">
+        <v>532</v>
+      </c>
+      <c r="C426"/>
+      <c r="D426" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="427" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B427" s="11" t="s">
+        <v>533</v>
+      </c>
+      <c r="C427"/>
+      <c r="D427" s="11" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="428" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B428" s="11"/>
-      <c r="C428" s="12"/>
-      <c r="D428" s="11"/>
-    </row>
-    <row r="429" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B429" s="11"/>
-      <c r="C429" s="12"/>
-      <c r="D429" s="11"/>
+      <c r="B428" s="11" t="s">
+        <v>534</v>
+      </c>
+      <c r="C428"/>
+      <c r="D428" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="429" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B429" s="11" t="s">
+        <v>535</v>
+      </c>
+      <c r="C429"/>
+      <c r="D429" s="11" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="430" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B430" s="11"/>
-      <c r="C430" s="12"/>
-      <c r="D430" s="11"/>
-    </row>
-    <row r="431" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B431" s="11"/>
-      <c r="C431" s="12"/>
-      <c r="D431" s="11"/>
+      <c r="B430" s="11" t="s">
+        <v>536</v>
+      </c>
+      <c r="C430"/>
+      <c r="D430" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="431" spans="2:4" ht="30.75" thickBot="1">
+      <c r="B431" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="C431"/>
+      <c r="D431" s="11" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="432" spans="2:4" ht="15.75" thickBot="1">
       <c r="B432" s="11"/>

</xml_diff>